<commit_message>
fill test excel file
</commit_message>
<xml_diff>
--- a/hw_2/module_4_task_2.xlsx
+++ b/hw_2/module_4_task_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krish\Desktop\1\module_testing\hw_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC1234A5-F6A6-4D7F-A395-A116DA6458D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B920226A-086C-4032-84AC-CBBC506F0782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{0861009E-620E-42F4-A7CE-5A21C66E0B2F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{0861009E-620E-42F4-A7CE-5A21C66E0B2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Среднее значение" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="94">
   <si>
     <t>Идентификатор теста</t>
   </si>
@@ -312,6 +312,12 @@
   </si>
   <si>
     <t>Вызвать функцию и передать список содержащий 1000 элементов</t>
+  </si>
+  <si>
+    <t>TypeError</t>
+  </si>
+  <si>
+    <t>PASSED</t>
   </si>
 </sst>
 </file>
@@ -319,7 +325,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="#,##0.0"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -364,12 +370,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9999"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -399,7 +417,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -421,15 +439,21 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -438,6 +462,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF9999"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -748,8 +777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2155770F-9ACB-4763-AABA-BE2D6CD206B5}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -810,458 +839,538 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="10">
         <f>AVERAGE(1, 2, 3)</f>
         <v>2</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
+      <c r="G7" s="10">
+        <v>2</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="10">
         <f>AVERAGE(-1, -2, -3)</f>
         <v>-2</v>
       </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
+      <c r="G8" s="10">
+        <v>-2</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>41</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="10">
         <f>AVERAGE(-1, 2, -3)</f>
         <v>-0.66666666666666663</v>
       </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
+      <c r="G9" s="10">
+        <v>-0.66666666666666663</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="10">
         <f>AVERAGE(0, 0, 0)</f>
         <v>0</v>
       </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
+      <c r="G10" s="10">
+        <v>0</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="8" t="s">
         <v>42</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="10">
         <f>AVERAGE(1, 0, 3)</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
+      <c r="G11" s="10">
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="12" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="8" t="s">
         <v>43</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="10">
         <f>AVERAGE(-1, 0, -3)</f>
         <v>-1.3333333333333333</v>
       </c>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
+      <c r="G12" s="10">
+        <v>-1.3333333333333333</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="13" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="8" t="s">
         <v>17</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="10">
         <f>AVERAGE(1, 1, 1)</f>
         <v>1</v>
       </c>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
+      <c r="G13" s="10">
+        <v>1</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="8" t="s">
         <v>82</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="10">
         <f>AVERAGE(3, 2, 1)</f>
         <v>2</v>
       </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+      <c r="G14" s="10">
+        <v>2</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="15" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="8" t="s">
         <v>83</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="10">
         <f>AVERAGE(1, 2, 3)</f>
         <v>2</v>
       </c>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
+      <c r="G15" s="10">
+        <v>2</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="16" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="8" t="s">
         <v>40</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="10">
         <f>AVERAGE(1, 100000, 2, 100000000)</f>
         <v>25025000.75</v>
       </c>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
+      <c r="G16" s="10">
+        <v>25025000.75</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="17" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="8" t="s">
         <v>15</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="10">
         <f>AVERAGE(1, 2.5, 3.9)</f>
         <v>2.4666666666666668</v>
       </c>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
+      <c r="G17" s="10">
+        <v>2.4666666666666668</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="18" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="8" t="s">
         <v>16</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="10">
         <f>AVERAGE(1, 2, 3)</f>
         <v>2</v>
       </c>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
+      <c r="G18" s="10">
+        <v>2</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="19" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="8" t="s">
         <v>38</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F19" s="10">
         <f>AVERAGE(1, 2.5, 3)</f>
         <v>2.1666666666666665</v>
       </c>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
+      <c r="G19" s="10">
+        <v>2.1666666666666665</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="20" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="8" t="s">
         <v>18</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="F20" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
+      <c r="F20" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="21" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="8" t="s">
         <v>39</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="F21" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
+      <c r="F21" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="22" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="8" t="s">
         <v>84</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="E22" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="F22" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
+      <c r="F22" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="23" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="8" t="s">
         <v>85</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E23" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="F23" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
+      <c r="F23" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="24" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="8" t="s">
         <v>86</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="E24" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="F24" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
+      <c r="G24" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="25" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="8" t="s">
         <v>87</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="E25" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="F25" s="11">
+      <c r="F25" s="10">
         <f>AVERAGE(1)</f>
         <v>1</v>
       </c>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
+      <c r="G25" s="10">
+        <v>1</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="26" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="8" t="s">
         <v>88</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E26" s="9" t="s">
+      <c r="E26" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="F26" s="11" t="s">
+      <c r="F26" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
+      <c r="G26" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>93</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>